<commit_message>
Prepravljen scenarij 1 i dodane skice prototipa.
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Scenarij/placanje putovanja.xlsx
+++ b/UseCaseIScenarij/Scenarij/placanje putovanja.xlsx
@@ -73,21 +73,6 @@
     <t>6.Registracija</t>
   </si>
   <si>
-    <t>6.Log in</t>
-  </si>
-  <si>
-    <t>7.Validacija log in</t>
-  </si>
-  <si>
-    <t>8.Odabir okvirnog termina putovanja</t>
-  </si>
-  <si>
-    <t>9.Prikaz mogucih termina</t>
-  </si>
-  <si>
-    <t>10.Odabir termina</t>
-  </si>
-  <si>
     <t>11.Obracun cijene</t>
   </si>
   <si>
@@ -146,6 +131,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>6.Odabir okvirnog termina putovanja</t>
+  </si>
+  <si>
+    <t>7.Prikaz mogucih termina</t>
+  </si>
+  <si>
+    <t>8.Odabir termina</t>
+  </si>
+  <si>
+    <t>9.Log in</t>
+  </si>
+  <si>
+    <t>10.Validacija Log in</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -298,50 +298,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,6 +318,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,71 +697,71 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
@@ -751,27 +769,27 @@
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -779,8 +797,8 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" s="6"/>
@@ -790,280 +808,336 @@
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="8"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="8"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="8"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23" t="s">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="8"/>
       <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="11" t="s">
+      <c r="F24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="25"/>
+    <row r="26" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="34"/>
       <c r="E26" s="8"/>
       <c r="F26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
+    <row r="27" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="8"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
+    <row r="28" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="8"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+    <row r="29" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+    <row r="30" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="3"/>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+    <row r="31" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="28"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="38"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="36"/>
       <c r="E33" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="36"/>
       <c r="E34" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
+      <c r="B38" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20" t="s">
+      <c r="B40" s="27"/>
+      <c r="C40" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="20"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="19"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="3"/>
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
+      <c r="A42" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="3"/>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="7" t="s">
         <v>17</v>
       </c>
@@ -1076,61 +1150,61 @@
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
+      <c r="A46" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20" t="s">
+      <c r="B48" s="27"/>
+      <c r="C48" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="20"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
+      <c r="A50" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="27"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,71 +1215,71 @@
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="31"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="56" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
+      <c r="A56" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20" t="s">
+      <c r="B57" s="27"/>
+      <c r="C57" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="20"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="23" t="s">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="23"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
       <c r="E60" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G60" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="33"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="21"/>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="37"/>
+      <c r="B62" s="25"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
@@ -1214,67 +1288,17 @@
       <c r="A64" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A2:A7"/>
+  <mergeCells count="86">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B2:E7"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C24:D24"/>
@@ -1291,6 +1315,66 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="C40:D40"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B2:E7"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>